<commit_message>
last changes I m done
</commit_message>
<xml_diff>
--- a/simulation_results_case2a.xlsx
+++ b/simulation_results_case2a.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk.sharepoint.com/sites/CITLResearchGroup/Delte dokumenter/General/09 - Personal/Alexandros/MUDP/Development/Digital_Twin_for_emissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_46FFFF80FBADC0ABA9144E10438E21C37198AAE5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BC62ABF-560D-4D38-B63F-E7B68DFF679D}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="11_46FFFF80FBADC0ABA9144E10438E21C37198AAE5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98A6C863-3E06-4307-9EE5-88DB0B7A1F54}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Truck Data" sheetId="1" r:id="rId1"/>
@@ -1424,7 +1424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1530,9 +1530,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B110"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -2423,9 +2429,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B164"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
@@ -3742,6 +3754,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="37543332-2da3-439b-bc98-209254b30f00">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="830a31a7-89b5-416e-b6e5-e0fe14d58a94" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100D40B40838B1139498AAB1AE2830B4A9D" ma:contentTypeVersion="14" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="79d0be0e660dbfe1199aced984f6c20c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="37543332-2da3-439b-bc98-209254b30f00" xmlns:ns3="830a31a7-89b5-416e-b6e5-e0fe14d58a94" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ffb1d47b889e36d1b69e90153213741a" ns2:_="" ns3:_="">
     <xsd:import namespace="37543332-2da3-439b-bc98-209254b30f00"/>
@@ -3970,34 +4002,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="37543332-2da3-439b-bc98-209254b30f00">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="830a31a7-89b5-416e-b6e5-e0fe14d58a94" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93F4C05B-B4DB-4714-B425-ABDB06C2565B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3ED469B5-4736-4FE3-A1C4-89F8CC4FE1DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="37543332-2da3-439b-bc98-209254b30f00"/>
+    <ds:schemaRef ds:uri="830a31a7-89b5-416e-b6e5-e0fe14d58a94"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACEE62DA-F2B4-4BA3-9648-6D5F3F6CECC8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACEE62DA-F2B4-4BA3-9648-6D5F3F6CECC8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3ED469B5-4736-4FE3-A1C4-89F8CC4FE1DE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93F4C05B-B4DB-4714-B425-ABDB06C2565B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="37543332-2da3-439b-bc98-209254b30f00"/>
+    <ds:schemaRef ds:uri="830a31a7-89b5-416e-b6e5-e0fe14d58a94"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>